<commit_message>
version 03 for Angular and Express project- remove Javascript file, instead by TypeScript completedly
</commit_message>
<xml_diff>
--- a/RESTFul_API.xlsx
+++ b/RESTFul_API.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Website_NenThomBnC\Website_NenThomBnC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{620A8D48-707F-45B9-A31C-48B5D38EB7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0911C529-D878-4D4C-A74C-6E0FB72B437C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3DCBFBA-82F4-4982-9C95-CC18301E2A03}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E3DCBFBA-82F4-4982-9C95-CC18301E2A03}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Before" sheetId="1" r:id="rId1"/>
+    <sheet name="After" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
   <si>
     <t>URL Name</t>
   </si>
@@ -656,6 +658,20 @@
   </si>
   <si>
     <t>- BASE_URL</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">YES: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>/RequestGetCandleByFilter</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1007,13 +1023,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1022,124 +1038,130 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1478,8 +1500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B298AE69-CA4F-49F7-9C30-8E01EBFFF002}">
   <dimension ref="B1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -1499,410 +1521,410 @@
       </c>
     </row>
     <row r="2" spans="2:8" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="26" t="s">
+      <c r="D2" s="39"/>
+      <c r="E2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="31" t="s">
+      <c r="F2" s="39"/>
+      <c r="G2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="42" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="3" spans="2:8" s="2" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
     </row>
     <row r="4" spans="2:8" s="2" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="34" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="28" t="s">
         <v>75</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="36" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:8" s="2" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="28" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="8"/>
-      <c r="E6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="22"/>
+      <c r="E6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="18"/>
       <c r="G6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="34" t="s">
+      <c r="H6" s="23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="22"/>
+      <c r="E7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="18"/>
       <c r="G7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="23" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="22"/>
+      <c r="E8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="18"/>
       <c r="G8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="23" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="22"/>
+      <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="18"/>
       <c r="G9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="23" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="12" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="22"/>
+      <c r="E10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="18"/>
       <c r="G10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="25" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="22"/>
+      <c r="E11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="18"/>
       <c r="G11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="23" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D12" s="8"/>
-      <c r="E12" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="22"/>
+      <c r="E12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="18"/>
       <c r="G12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="H12" s="23" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="8"/>
-      <c r="E13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" s="22"/>
+      <c r="E13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="18"/>
       <c r="G13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="23" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="22"/>
+      <c r="E14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="18"/>
       <c r="G14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="34" t="s">
+      <c r="H14" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="22"/>
+      <c r="E15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="18"/>
       <c r="G15" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="34" t="s">
+      <c r="H15" s="23" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="32" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="12" t="s">
+      <c r="E16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="45" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
+      <c r="B17" s="32"/>
       <c r="C17" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="22"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="E17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
     </row>
     <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
+      <c r="B18" s="32"/>
       <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
       <c r="D18" s="8"/>
-      <c r="E18" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="22"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="E18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
     </row>
     <row r="19" spans="2:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="11"/>
+      <c r="B19" s="32"/>
       <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" s="22"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="E19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
     </row>
     <row r="20" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="47" t="s">
         <v>45</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="14" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="33" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
-      <c r="C21" s="13"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="47"/>
       <c r="D21" s="4"/>
       <c r="E21" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="2:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="47" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="14" t="s">
+      <c r="F22" s="19"/>
+      <c r="G22" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="36" t="s">
+      <c r="H22" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="11"/>
-      <c r="C23" s="13"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="47"/>
       <c r="D23" s="4"/>
       <c r="E23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="23"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
     </row>
     <row r="24" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>38</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="22"/>
+      <c r="E24" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="18"/>
       <c r="G24" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="H24" s="34" t="s">
+      <c r="H24" s="23" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="32" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -1912,16 +1934,16 @@
       <c r="E25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="24"/>
-      <c r="G25" s="14" t="s">
+      <c r="F25" s="20"/>
+      <c r="G25" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="33" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="258.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
+      <c r="B26" s="32"/>
       <c r="C26" s="8" t="s">
         <v>50</v>
       </c>
@@ -1929,61 +1951,62 @@
       <c r="E26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="24"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" spans="2:8" ht="258.60000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="44" t="s">
+      <c r="C27" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="45" t="s">
+      <c r="H27" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="15" t="s">
+      <c r="C28" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="21"/>
+      <c r="G28" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="37" t="s">
+      <c r="H28" s="24" t="s">
         <v>71</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="H25:H26"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G2:G3"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="H16:H19"/>
@@ -1994,7 +2017,544 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="G16:G19"/>
-    <mergeCell ref="G20:G21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30DBCCF6-47F2-4D3B-91D8-10A3CB0FE52D}">
+  <dimension ref="B1:H29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="3" width="32.44140625" customWidth="1"/>
+    <col min="4" max="4" width="111.33203125" customWidth="1"/>
+    <col min="5" max="6" width="91.6640625" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
+    <col min="8" max="8" width="66.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" s="2" customFormat="1" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="39"/>
+      <c r="E2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="39"/>
+      <c r="G2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="2" customFormat="1" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41"/>
+      <c r="C3" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="2:8" s="2" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="2" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="35"/>
+      <c r="C5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+    </row>
+    <row r="6" spans="2:8" s="2" customFormat="1" ht="176.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="32"/>
+      <c r="C18" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="32"/>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+    </row>
+    <row r="20" spans="2:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="32"/>
+      <c r="C20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+    </row>
+    <row r="21" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="32"/>
+      <c r="C22" s="47"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+    </row>
+    <row r="23" spans="2:8" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="32"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="258.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="32"/>
+      <c r="C27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+    </row>
+    <row r="28" spans="2:8" ht="258.60000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="21"/>
+      <c r="G29" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="B17:B20"/>
+    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="H17:H20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>